<commit_message>
Added the ability to insert information to files with min cost for product Samsung and and the prices of all remaining products Samsung.
</commit_message>
<xml_diff>
--- a/comfy_data.xlsx
+++ b/comfy_data.xlsx
@@ -747,7 +747,7 @@
     <t>https://comfy.ua/ua/</t>
   </si>
   <si>
-    <t>Серийный номер</t>
+    <t>Серійний номер</t>
   </si>
   <si>
     <t>SM-M325FZKGSEK</t>
@@ -1447,7 +1447,7 @@
   <dimension ref="A1:E143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added the ability to send emails using smtp.
</commit_message>
<xml_diff>
--- a/comfy_data.xlsx
+++ b/comfy_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="242">
   <si>
     <t>Назва</t>
   </si>
@@ -745,366 +745,6 @@
   </si>
   <si>
     <t>https://comfy.ua/ua/</t>
-  </si>
-  <si>
-    <t>Серійний номер</t>
-  </si>
-  <si>
-    <t>SM-M325FZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-A536EZKDSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BZAFSEK</t>
-  </si>
-  <si>
-    <t>SM-M135FZGDSEK</t>
-  </si>
-  <si>
-    <t>SM-A045FZKDSEK</t>
-  </si>
-  <si>
-    <t>SM-A336BZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-F721BLBHSEK</t>
-  </si>
-  <si>
-    <t>SM-A736BZADSEK</t>
-  </si>
-  <si>
-    <t>SM-A235FZKKSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-A536EZKHSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BZAWSEK</t>
-  </si>
-  <si>
-    <t>SM-M325FLBGSEK</t>
-  </si>
-  <si>
-    <t>SM-M325FZWGSEK</t>
-  </si>
-  <si>
-    <t>SM-M135FZGGSEK</t>
-  </si>
-  <si>
-    <t>SM-A536ELBHSEK</t>
-  </si>
-  <si>
-    <t>SM-A536EZOHSEK</t>
-  </si>
-  <si>
-    <t>SM-M135FIDGSEK</t>
-  </si>
-  <si>
-    <t>SM-M135FIDDSEK</t>
-  </si>
-  <si>
-    <t>SM-A536EZODSEK</t>
-  </si>
-  <si>
-    <t>SM-A536EZWHSEK</t>
-  </si>
-  <si>
-    <t>SM-A536EZWDSEK</t>
-  </si>
-  <si>
-    <t>SM-A536ELBDSEK</t>
-  </si>
-  <si>
-    <t>SM-M135FLBDSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FZKKSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FZKVSEK</t>
-  </si>
-  <si>
-    <t>SM-A035FZKDSEK</t>
-  </si>
-  <si>
-    <t>SM-A035FZBDSEK</t>
-  </si>
-  <si>
-    <t>SM-A235FZOKSEK</t>
-  </si>
-  <si>
-    <t>SM-A336BZOGSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FLBKSEK</t>
-  </si>
-  <si>
-    <t>SM-A035FZRDSEK</t>
-  </si>
-  <si>
-    <t>SM-A325FZKDSEK</t>
-  </si>
-  <si>
-    <t>SM-A325FZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-A325FLVGSEK</t>
-  </si>
-  <si>
-    <t>SM-M336BZNGSEK</t>
-  </si>
-  <si>
-    <t>SM-M336BZGGSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FLBUSEK</t>
-  </si>
-  <si>
-    <t>SM-M336BZBGSEK</t>
-  </si>
-  <si>
-    <t>SM-A736BZAHSEK</t>
-  </si>
-  <si>
-    <t>SM-A736BLGHSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FZKUSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FZWKSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BLVFSEK</t>
-  </si>
-  <si>
-    <t>SM-A325FZBDSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BLGFSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FLBVSEK</t>
-  </si>
-  <si>
-    <t>SM-A032FCKDSEK</t>
-  </si>
-  <si>
-    <t>SM-A032FLGDSEK</t>
-  </si>
-  <si>
-    <t>SM-A037FZKDSEK</t>
-  </si>
-  <si>
-    <t>SM-A035FZRGSEK</t>
-  </si>
-  <si>
-    <t>SM-A032FZCDSEK</t>
-  </si>
-  <si>
-    <t>SM-A037FZBDSEK</t>
-  </si>
-  <si>
-    <t>SM-A035FZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-A035FZBGSEK</t>
-  </si>
-  <si>
-    <t>SM-A037FZBGSEK</t>
-  </si>
-  <si>
-    <t>SM-A037FZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-A045FZGDSEK</t>
-  </si>
-  <si>
-    <t>SM-A045FZCDSEK</t>
-  </si>
-  <si>
-    <t>SM-A045FZGGSEK</t>
-  </si>
-  <si>
-    <t>SM-A045FZCGSEK</t>
-  </si>
-  <si>
-    <t>SM-A045FZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-A047FZGUSEK</t>
-  </si>
-  <si>
-    <t>SM-A047FZCUSEK</t>
-  </si>
-  <si>
-    <t>SM-A047FZKUSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FZWUSEK</t>
-  </si>
-  <si>
-    <t>SM-A047FZGVSEK</t>
-  </si>
-  <si>
-    <t>SM-A047FZCVSEK</t>
-  </si>
-  <si>
-    <t>SM-A047FZKVSEK</t>
-  </si>
-  <si>
-    <t>SM-A135FZWVSEK</t>
-  </si>
-  <si>
-    <t>SM-M135FLBGSEK</t>
-  </si>
-  <si>
-    <t>SM-A235FZKUSEK</t>
-  </si>
-  <si>
-    <t>SM-A235FZOUSEK</t>
-  </si>
-  <si>
-    <t>SM-A235FZWUSEK</t>
-  </si>
-  <si>
-    <t>SM-A235FZWKSEK</t>
-  </si>
-  <si>
-    <t>SM-A325FLVDSEK</t>
-  </si>
-  <si>
-    <t>SM-M236BLBDSEK</t>
-  </si>
-  <si>
-    <t>SM-M236BZGGSEK</t>
-  </si>
-  <si>
-    <t>SM-M236BLBGSEK</t>
-  </si>
-  <si>
-    <t>SM-A336BZWGSEK</t>
-  </si>
-  <si>
-    <t>SM-A336BLBGSEK</t>
-  </si>
-  <si>
-    <t>SM-M536BZGDSEK</t>
-  </si>
-  <si>
-    <t>SM-M536BZBDSEK</t>
-  </si>
-  <si>
-    <t>SM-M536BZNDSEK</t>
-  </si>
-  <si>
-    <t>SM-A736BZWDSEK</t>
-  </si>
-  <si>
-    <t>SM-A736BLGDSEK</t>
-  </si>
-  <si>
-    <t>SM-A736BZWHSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BZWFSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BLVWSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BZWWSEK</t>
-  </si>
-  <si>
-    <t>SM-G990BLGWSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BIDDSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BZGDSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BZWDSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BLVDSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BZKDSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BZWGSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BLVGSEK</t>
-  </si>
-  <si>
-    <t>SM-S901BIDGSEK</t>
-  </si>
-  <si>
-    <t>SM-S906BIDDSEK</t>
-  </si>
-  <si>
-    <t>SM-S906BZKDSEK</t>
-  </si>
-  <si>
-    <t>SM-S906BZGDSEK</t>
-  </si>
-  <si>
-    <t>SM-F721BZAHSEK</t>
-  </si>
-  <si>
-    <t>SM-F721BLVHSEK</t>
-  </si>
-  <si>
-    <t>SM-S906BZGGSEK</t>
-  </si>
-  <si>
-    <t>SM-S906BZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-S906BZWGSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BDRDSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BZGDSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BZWDSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BDRGSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BZGGSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BZKGSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BZWGSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BZKHSEK</t>
-  </si>
-  <si>
-    <t>SM-S908BDRHSEK</t>
-  </si>
-  <si>
-    <t>SM-F936BZKBSEK</t>
-  </si>
-  <si>
-    <t>SM-F936BZACSEK</t>
-  </si>
-  <si>
-    <t>SM-F936BZKCSEK</t>
   </si>
 </sst>
 </file>
@@ -1444,18 +1084,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E143"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="5" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1468,11 +1108,8 @@
       <c r="D1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1485,11 +1122,8 @@
       <c r="D2" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1502,11 +1136,8 @@
       <c r="D3" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1519,11 +1150,8 @@
       <c r="D4" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1536,11 +1164,8 @@
       <c r="D5" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1553,11 +1178,8 @@
       <c r="D6" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1570,11 +1192,8 @@
       <c r="D7" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1587,11 +1206,8 @@
       <c r="D8" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1604,11 +1220,8 @@
       <c r="D9" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1621,11 +1234,8 @@
       <c r="D10" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1638,11 +1248,8 @@
       <c r="D11" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1655,11 +1262,8 @@
       <c r="D12" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1672,11 +1276,8 @@
       <c r="D13" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1689,11 +1290,8 @@
       <c r="D14" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1706,11 +1304,8 @@
       <c r="D15" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1723,11 +1318,8 @@
       <c r="D16" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1740,11 +1332,8 @@
       <c r="D17" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1757,11 +1346,8 @@
       <c r="D18" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1774,11 +1360,8 @@
       <c r="D19" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1791,11 +1374,8 @@
       <c r="D20" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1808,11 +1388,8 @@
       <c r="D21" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -1825,11 +1402,8 @@
       <c r="D22" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1842,11 +1416,8 @@
       <c r="D23" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1859,11 +1430,8 @@
       <c r="D24" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1876,11 +1444,8 @@
       <c r="D25" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1893,11 +1458,8 @@
       <c r="D26" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1910,11 +1472,8 @@
       <c r="D27" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1927,11 +1486,8 @@
       <c r="D28" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1944,11 +1500,8 @@
       <c r="D29" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1961,11 +1514,8 @@
       <c r="D30" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1978,11 +1528,8 @@
       <c r="D31" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1995,11 +1542,8 @@
       <c r="D32" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2012,11 +1556,8 @@
       <c r="D33" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -2029,11 +1570,8 @@
       <c r="D34" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -2046,11 +1584,8 @@
       <c r="D35" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -2063,11 +1598,8 @@
       <c r="D36" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -2080,11 +1612,8 @@
       <c r="D37" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -2097,11 +1626,8 @@
       <c r="D38" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -2114,11 +1640,8 @@
       <c r="D39" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -2131,11 +1654,8 @@
       <c r="D40" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>81</v>
       </c>
@@ -2148,11 +1668,8 @@
       <c r="D41" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>83</v>
       </c>
@@ -2165,11 +1682,8 @@
       <c r="D42" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -2182,11 +1696,8 @@
       <c r="D43" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -2199,11 +1710,8 @@
       <c r="D44" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2216,11 +1724,8 @@
       <c r="D45" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>91</v>
       </c>
@@ -2233,11 +1738,8 @@
       <c r="D46" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>93</v>
       </c>
@@ -2250,11 +1752,8 @@
       <c r="D47" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -2267,11 +1766,8 @@
       <c r="D48" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -2284,11 +1780,8 @@
       <c r="D49" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -2301,11 +1794,8 @@
       <c r="D50" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>101</v>
       </c>
@@ -2318,11 +1808,8 @@
       <c r="D51" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>103</v>
       </c>
@@ -2335,11 +1822,8 @@
       <c r="D52" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>105</v>
       </c>
@@ -2352,11 +1836,8 @@
       <c r="D53" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>107</v>
       </c>
@@ -2369,11 +1850,8 @@
       <c r="D54" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>109</v>
       </c>
@@ -2386,11 +1864,8 @@
       <c r="D55" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>111</v>
       </c>
@@ -2403,11 +1878,8 @@
       <c r="D56" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>113</v>
       </c>
@@ -2420,11 +1892,8 @@
       <c r="D57" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>115</v>
       </c>
@@ -2437,11 +1906,8 @@
       <c r="D58" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>117</v>
       </c>
@@ -2454,11 +1920,8 @@
       <c r="D59" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -2471,11 +1934,8 @@
       <c r="D60" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -2488,11 +1948,8 @@
       <c r="D61" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>123</v>
       </c>
@@ -2505,11 +1962,8 @@
       <c r="D62" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>125</v>
       </c>
@@ -2522,11 +1976,8 @@
       <c r="D63" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>127</v>
       </c>
@@ -2539,11 +1990,8 @@
       <c r="D64" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>129</v>
       </c>
@@ -2556,11 +2004,8 @@
       <c r="D65" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>131</v>
       </c>
@@ -2573,11 +2018,8 @@
       <c r="D66" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>133</v>
       </c>
@@ -2590,11 +2032,8 @@
       <c r="D67" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -2607,11 +2046,8 @@
       <c r="D68" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>137</v>
       </c>
@@ -2624,11 +2060,8 @@
       <c r="D69" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>139</v>
       </c>
@@ -2641,11 +2074,8 @@
       <c r="D70" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>141</v>
       </c>
@@ -2658,11 +2088,8 @@
       <c r="D71" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>143</v>
       </c>
@@ -2675,11 +2102,8 @@
       <c r="D72" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>145</v>
       </c>
@@ -2692,11 +2116,8 @@
       <c r="D73" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>147</v>
       </c>
@@ -2709,11 +2130,8 @@
       <c r="D74" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>149</v>
       </c>
@@ -2726,11 +2144,8 @@
       <c r="D75" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>151</v>
       </c>
@@ -2743,11 +2158,8 @@
       <c r="D76" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E76" s="1" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>153</v>
       </c>
@@ -2760,11 +2172,8 @@
       <c r="D77" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>155</v>
       </c>
@@ -2777,11 +2186,8 @@
       <c r="D78" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>157</v>
       </c>
@@ -2794,11 +2200,8 @@
       <c r="D79" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>159</v>
       </c>
@@ -2811,11 +2214,8 @@
       <c r="D80" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>161</v>
       </c>
@@ -2828,11 +2228,8 @@
       <c r="D81" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>163</v>
       </c>
@@ -2845,11 +2242,8 @@
       <c r="D82" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>165</v>
       </c>
@@ -2862,11 +2256,8 @@
       <c r="D83" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>167</v>
       </c>
@@ -2879,11 +2270,8 @@
       <c r="D84" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E84" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>169</v>
       </c>
@@ -2896,11 +2284,8 @@
       <c r="D85" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>171</v>
       </c>
@@ -2913,11 +2298,8 @@
       <c r="D86" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>173</v>
       </c>
@@ -2930,11 +2312,8 @@
       <c r="D87" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>175</v>
       </c>
@@ -2947,11 +2326,8 @@
       <c r="D88" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>177</v>
       </c>
@@ -2964,11 +2340,8 @@
       <c r="D89" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>179</v>
       </c>
@@ -2981,11 +2354,8 @@
       <c r="D90" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>181</v>
       </c>
@@ -2998,11 +2368,8 @@
       <c r="D91" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E91" s="1" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>183</v>
       </c>
@@ -3015,11 +2382,8 @@
       <c r="D92" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>185</v>
       </c>
@@ -3032,11 +2396,8 @@
       <c r="D93" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>187</v>
       </c>
@@ -3049,11 +2410,8 @@
       <c r="D94" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>189</v>
       </c>
@@ -3066,11 +2424,8 @@
       <c r="D95" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>191</v>
       </c>
@@ -3083,11 +2438,8 @@
       <c r="D96" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>193</v>
       </c>
@@ -3100,11 +2452,8 @@
       <c r="D97" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>195</v>
       </c>
@@ -3117,11 +2466,8 @@
       <c r="D98" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>197</v>
       </c>
@@ -3134,11 +2480,8 @@
       <c r="D99" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>199</v>
       </c>
@@ -3151,11 +2494,8 @@
       <c r="D100" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>201</v>
       </c>
@@ -3168,11 +2508,8 @@
       <c r="D101" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>203</v>
       </c>
@@ -3185,11 +2522,8 @@
       <c r="D102" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>205</v>
       </c>
@@ -3202,11 +2536,8 @@
       <c r="D103" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>207</v>
       </c>
@@ -3219,11 +2550,8 @@
       <c r="D104" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E104" s="1" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>209</v>
       </c>
@@ -3236,11 +2564,8 @@
       <c r="D105" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>211</v>
       </c>
@@ -3253,11 +2578,8 @@
       <c r="D106" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E106" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>213</v>
       </c>
@@ -3270,11 +2592,8 @@
       <c r="D107" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E107" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>215</v>
       </c>
@@ -3287,11 +2606,8 @@
       <c r="D108" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>217</v>
       </c>
@@ -3304,11 +2620,8 @@
       <c r="D109" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E109" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>219</v>
       </c>
@@ -3321,11 +2634,8 @@
       <c r="D110" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>221</v>
       </c>
@@ -3338,11 +2648,8 @@
       <c r="D111" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>223</v>
       </c>
@@ -3355,11 +2662,8 @@
       <c r="D112" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>225</v>
       </c>
@@ -3372,11 +2676,8 @@
       <c r="D113" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>227</v>
       </c>
@@ -3389,11 +2690,8 @@
       <c r="D114" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>229</v>
       </c>
@@ -3406,11 +2704,8 @@
       <c r="D115" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E115" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>231</v>
       </c>
@@ -3423,11 +2718,8 @@
       <c r="D116" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E116" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>233</v>
       </c>
@@ -3440,11 +2732,8 @@
       <c r="D117" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E117" s="1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>235</v>
       </c>
@@ -3457,11 +2746,8 @@
       <c r="D118" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E118" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>237</v>
       </c>
@@ -3474,11 +2760,8 @@
       <c r="D119" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>239</v>
       </c>
@@ -3488,11 +2771,8 @@
       <c r="D120" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B121">
         <v>4299</v>
       </c>
@@ -3500,7 +2780,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B122">
         <v>4299</v>
       </c>
@@ -3508,7 +2788,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B123">
         <v>4299</v>
       </c>
@@ -3516,7 +2796,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B124">
         <v>4399</v>
       </c>
@@ -3524,7 +2804,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B125">
         <v>4999</v>
       </c>
@@ -3532,7 +2812,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B126">
         <v>4999</v>
       </c>
@@ -3540,7 +2820,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B127">
         <v>4999</v>
       </c>
@@ -3548,7 +2828,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>4999</v>
       </c>

</xml_diff>